<commit_message>
started the data cleaning process and coding
</commit_message>
<xml_diff>
--- a/data/class_action_filings.xlsx
+++ b/data/class_action_filings.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pdoyle/school/capstone/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5590E594-1D40-E744-9E69-2C555FDC197D}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68469A35-D3FC-6946-A57C-8C29950A541D}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="47260" yWindow="8600" windowWidth="23860" windowHeight="27760" xr2:uid="{8A99C31B-3B6B-354D-8DFC-65D08A4662CA}"/>
   </bookViews>
@@ -553,8 +553,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{784FBB69-F05A-8347-8200-5F5BF64288D8}">
   <dimension ref="A1:E59"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="142" zoomScaleNormal="142" workbookViewId="0">
-      <selection activeCell="D42" sqref="D42"/>
+    <sheetView tabSelected="1" zoomScale="142" zoomScaleNormal="142" workbookViewId="0">
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -623,6 +623,9 @@
       <c r="D4" t="s">
         <v>8</v>
       </c>
+      <c r="E4" s="2">
+        <v>0</v>
+      </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" t="s">

</xml_diff>

<commit_message>
Added comments to funtions in import_data.R
</commit_message>
<xml_diff>
--- a/data/class_action_filings.xlsx
+++ b/data/class_action_filings.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pdoyle/school/capstone/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68469A35-D3FC-6946-A57C-8C29950A541D}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67E29059-B51C-F44B-8E77-1BF93C1A5F4E}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="47260" yWindow="8600" windowWidth="23860" windowHeight="27760" xr2:uid="{8A99C31B-3B6B-354D-8DFC-65D08A4662CA}"/>
+    <workbookView xWindow="8720" yWindow="960" windowWidth="23860" windowHeight="19140" xr2:uid="{8A99C31B-3B6B-354D-8DFC-65D08A4662CA}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="52">
   <si>
     <t>tic</t>
   </si>
@@ -551,10 +551,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{784FBB69-F05A-8347-8200-5F5BF64288D8}">
-  <dimension ref="A1:E59"/>
+  <dimension ref="A1:E58"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="142" zoomScaleNormal="142" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection activeCell="E25" sqref="E25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -666,16 +666,16 @@
         <v>20</v>
       </c>
       <c r="B7" s="1">
-        <v>42695</v>
+        <v>41358</v>
       </c>
       <c r="C7" s="1">
-        <v>43222</v>
+        <v>42144</v>
       </c>
       <c r="D7" t="s">
         <v>5</v>
       </c>
       <c r="E7" s="2">
-        <v>1300000</v>
+        <v>2600000</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
@@ -683,16 +683,16 @@
         <v>20</v>
       </c>
       <c r="B8" s="1">
-        <v>41358</v>
+        <v>42695</v>
       </c>
       <c r="C8" s="1">
-        <v>42144</v>
+        <v>43222</v>
       </c>
       <c r="D8" t="s">
         <v>5</v>
       </c>
       <c r="E8" s="2">
-        <v>2600000</v>
+        <v>1300000</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
@@ -717,16 +717,16 @@
         <v>7</v>
       </c>
       <c r="B10" s="1">
-        <v>42716</v>
+        <v>37092</v>
       </c>
       <c r="C10" s="1">
-        <v>43098</v>
+        <v>40092</v>
       </c>
       <c r="D10" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="E10" s="2">
-        <v>0</v>
+        <v>7000000</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
@@ -751,16 +751,16 @@
         <v>7</v>
       </c>
       <c r="B12" s="1">
-        <v>37092</v>
+        <v>42716</v>
       </c>
       <c r="C12" s="1">
-        <v>40092</v>
+        <v>43098</v>
       </c>
       <c r="D12" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="E12" s="2">
-        <v>7000000</v>
+        <v>0</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
@@ -768,16 +768,16 @@
         <v>22</v>
       </c>
       <c r="B13" s="1">
-        <v>41114</v>
+        <v>36322</v>
       </c>
       <c r="C13" s="1">
-        <v>41395</v>
+        <v>37011</v>
       </c>
       <c r="D13" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="E13" s="2">
-        <v>10000000</v>
+        <v>0</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
@@ -785,27 +785,27 @@
         <v>22</v>
       </c>
       <c r="B14" s="1">
-        <v>37224</v>
+        <v>41114</v>
       </c>
       <c r="C14" s="1">
-        <v>37820</v>
+        <v>41395</v>
       </c>
       <c r="D14" t="s">
         <v>5</v>
       </c>
       <c r="E14" s="2">
-        <v>450000</v>
+        <v>10000000</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B15" s="1">
-        <v>36322</v>
+        <v>42034</v>
       </c>
       <c r="C15" s="1">
-        <v>37011</v>
+        <v>42201</v>
       </c>
       <c r="D15" t="s">
         <v>8</v>
@@ -816,13 +816,13 @@
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B16" s="1">
-        <v>42034</v>
+        <v>36033</v>
       </c>
       <c r="C16" s="1">
-        <v>42201</v>
+        <v>36661</v>
       </c>
       <c r="D16" t="s">
         <v>8</v>
@@ -833,13 +833,13 @@
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>24</v>
+        <v>9</v>
       </c>
       <c r="B17" s="1">
-        <v>36033</v>
+        <v>42319</v>
       </c>
       <c r="C17" s="1">
-        <v>36661</v>
+        <v>42761</v>
       </c>
       <c r="D17" t="s">
         <v>8</v>
@@ -867,81 +867,81 @@
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="B19" s="1">
-        <v>42319</v>
+        <v>39094</v>
       </c>
       <c r="C19" s="1">
-        <v>42761</v>
+        <v>42253</v>
       </c>
       <c r="D19" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="E19" s="2">
-        <v>0</v>
+        <v>30000000</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>4</v>
+        <v>25</v>
       </c>
       <c r="B20" s="1">
-        <v>39094</v>
+        <v>38496</v>
       </c>
       <c r="C20" s="1">
-        <v>42253</v>
+        <v>38835</v>
       </c>
       <c r="D20" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="E20" s="2">
-        <v>30000000</v>
+        <v>0</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B21" s="1">
-        <v>38496</v>
+        <v>36766</v>
       </c>
       <c r="C21" s="1">
-        <v>38835</v>
+        <v>38545</v>
       </c>
       <c r="D21" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="E21" s="2">
-        <v>0</v>
+        <v>4350000</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B22" s="1">
-        <v>36766</v>
+        <v>39759</v>
       </c>
       <c r="C22" s="1">
-        <v>38545</v>
+        <v>40372</v>
       </c>
       <c r="D22" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="E22" s="2">
-        <v>4350000</v>
+        <v>0</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B23" s="1">
-        <v>39759</v>
+        <v>38699</v>
       </c>
       <c r="C23" s="1">
-        <v>40372</v>
+        <v>39682</v>
       </c>
       <c r="D23" t="s">
         <v>8</v>
@@ -969,44 +969,44 @@
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B25" s="1">
-        <v>38699</v>
+        <v>42167</v>
       </c>
       <c r="C25" s="1">
-        <v>39682</v>
+        <v>43276</v>
       </c>
       <c r="D25" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="E25" s="2">
-        <v>0</v>
+        <v>50000000</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B26" s="1">
-        <v>42167</v>
+        <v>38973</v>
       </c>
       <c r="C26" s="1">
-        <v>43276</v>
+        <v>41792</v>
       </c>
       <c r="D26" t="s">
         <v>5</v>
       </c>
       <c r="E26" s="2">
-        <v>50000000</v>
+        <v>40000000</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>10</v>
+        <v>30</v>
       </c>
       <c r="B27" s="1">
-        <v>43228</v>
+        <v>41780</v>
       </c>
       <c r="D27" t="s">
         <v>11</v>
@@ -1014,30 +1014,30 @@
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>10</v>
+        <v>31</v>
       </c>
       <c r="B28" s="1">
-        <v>37419</v>
+        <v>42304</v>
       </c>
       <c r="C28" s="1">
-        <v>38293</v>
+        <v>42669</v>
       </c>
       <c r="D28" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="E28" s="2">
-        <v>23000000</v>
+        <v>0</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>12</v>
+        <v>32</v>
       </c>
       <c r="B29" s="1">
-        <v>42968</v>
+        <v>39805</v>
       </c>
       <c r="C29" s="1">
-        <v>43004</v>
+        <v>41180</v>
       </c>
       <c r="D29" t="s">
         <v>8</v>
@@ -1048,55 +1048,61 @@
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>12</v>
+        <v>33</v>
       </c>
       <c r="B30" s="1">
-        <v>39462</v>
+        <v>39384</v>
       </c>
       <c r="C30" s="1">
-        <v>40469</v>
+        <v>40122</v>
       </c>
       <c r="D30" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="E30" s="2">
-        <v>3000000</v>
+        <v>0</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>13</v>
+        <v>34</v>
       </c>
       <c r="B31" s="1">
-        <v>42999</v>
+        <v>37222</v>
+      </c>
+      <c r="C31" s="1">
+        <v>40092</v>
       </c>
       <c r="D31" t="s">
-        <v>11</v>
+        <v>5</v>
+      </c>
+      <c r="E31" s="2">
+        <v>10800000</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>14</v>
+        <v>35</v>
       </c>
       <c r="B32" s="1">
-        <v>36826</v>
+        <v>37109</v>
       </c>
       <c r="C32" s="1">
-        <v>37797</v>
+        <v>40092</v>
       </c>
       <c r="D32" t="s">
         <v>5</v>
       </c>
       <c r="E32" s="2">
-        <v>4000000</v>
+        <v>0</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="B33" s="1">
-        <v>41780</v>
+        <v>42300</v>
       </c>
       <c r="D33" t="s">
         <v>11</v>
@@ -1104,30 +1110,30 @@
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>30</v>
+        <v>36</v>
       </c>
       <c r="B34" s="1">
-        <v>38973</v>
+        <v>38692</v>
       </c>
       <c r="C34" s="1">
-        <v>41792</v>
+        <v>39505</v>
       </c>
       <c r="D34" t="s">
         <v>5</v>
       </c>
       <c r="E34" s="2">
-        <v>40000000</v>
+        <v>6875000</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>31</v>
+        <v>37</v>
       </c>
       <c r="B35" s="1">
-        <v>42304</v>
+        <v>38969</v>
       </c>
       <c r="C35" s="1">
-        <v>42669</v>
+        <v>43160</v>
       </c>
       <c r="D35" t="s">
         <v>8</v>
@@ -1138,109 +1144,109 @@
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>32</v>
+        <v>10</v>
       </c>
       <c r="B36" s="1">
-        <v>39805</v>
+        <v>37419</v>
       </c>
       <c r="C36" s="1">
-        <v>41180</v>
+        <v>38293</v>
       </c>
       <c r="D36" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="E36" s="2">
-        <v>0</v>
+        <v>23000000</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>33</v>
+        <v>10</v>
       </c>
       <c r="B37" s="1">
-        <v>39384</v>
-      </c>
-      <c r="C37" s="1">
-        <v>40122</v>
+        <v>43228</v>
       </c>
       <c r="D37" t="s">
-        <v>8</v>
-      </c>
-      <c r="E37" s="2">
-        <v>0</v>
+        <v>11</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="B38" s="1">
-        <v>37222</v>
+        <v>36598</v>
       </c>
       <c r="C38" s="1">
-        <v>40092</v>
+        <v>36984</v>
       </c>
       <c r="D38" t="s">
         <v>5</v>
       </c>
       <c r="E38" s="2">
-        <v>10800000</v>
+        <v>6000000</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="B39" s="1">
-        <v>42300</v>
+        <v>38748</v>
+      </c>
+      <c r="C39" s="1">
+        <v>39952</v>
       </c>
       <c r="D39" t="s">
-        <v>11</v>
+        <v>8</v>
+      </c>
+      <c r="E39" s="2">
+        <v>0</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>35</v>
+        <v>40</v>
       </c>
       <c r="B40" s="1">
-        <v>37109</v>
+        <v>36705</v>
       </c>
       <c r="C40" s="1">
-        <v>40092</v>
+        <v>40115</v>
       </c>
       <c r="D40" t="s">
         <v>5</v>
       </c>
       <c r="E40" s="2">
-        <v>0</v>
+        <v>16400000</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>36</v>
+        <v>41</v>
       </c>
       <c r="B41" s="1">
-        <v>38692</v>
+        <v>41453</v>
       </c>
       <c r="C41" s="1">
-        <v>39505</v>
+        <v>41894</v>
       </c>
       <c r="D41" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="E41" s="2">
-        <v>6875000</v>
+        <v>0</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>37</v>
+        <v>42</v>
       </c>
       <c r="B42" s="1">
-        <v>38969</v>
+        <v>39298</v>
       </c>
       <c r="C42" s="1">
-        <v>43160</v>
+        <v>39294</v>
       </c>
       <c r="D42" t="s">
         <v>8</v>
@@ -1251,30 +1257,30 @@
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>38</v>
+        <v>43</v>
       </c>
       <c r="B43" s="1">
-        <v>36598</v>
+        <v>36976</v>
       </c>
       <c r="C43" s="1">
-        <v>36984</v>
+        <v>37529</v>
       </c>
       <c r="D43" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="E43" s="2">
-        <v>6000000</v>
+        <v>0</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>39</v>
+        <v>44</v>
       </c>
       <c r="B44" s="1">
-        <v>38748</v>
+        <v>40686</v>
       </c>
       <c r="C44" s="1">
-        <v>39952</v>
+        <v>41180</v>
       </c>
       <c r="D44" t="s">
         <v>8</v>
@@ -1285,47 +1291,47 @@
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>40</v>
+        <v>45</v>
       </c>
       <c r="B45" s="1">
-        <v>36705</v>
+        <v>42873</v>
       </c>
       <c r="C45" s="1">
-        <v>40115</v>
+        <v>42951</v>
       </c>
       <c r="D45" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="E45" s="2">
-        <v>16400000</v>
+        <v>0</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
       <c r="B46" s="1">
-        <v>41453</v>
+        <v>38413</v>
       </c>
       <c r="C46" s="1">
-        <v>41894</v>
+        <v>39146</v>
       </c>
       <c r="D46" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="E46" s="2">
-        <v>0</v>
+        <v>11000000</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>42</v>
+        <v>47</v>
       </c>
       <c r="B47" s="1">
-        <v>39298</v>
+        <v>38083</v>
       </c>
       <c r="C47" s="1">
-        <v>39294</v>
+        <v>38807</v>
       </c>
       <c r="D47" t="s">
         <v>8</v>
@@ -1336,13 +1342,13 @@
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="B48" s="1">
-        <v>36976</v>
+        <v>40214</v>
       </c>
       <c r="C48" s="1">
-        <v>37529</v>
+        <v>40890</v>
       </c>
       <c r="D48" t="s">
         <v>8</v>
@@ -1353,13 +1359,13 @@
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="B49" s="1">
-        <v>40686</v>
+        <v>41032</v>
       </c>
       <c r="C49" s="1">
-        <v>41180</v>
+        <v>41255</v>
       </c>
       <c r="D49" t="s">
         <v>8</v>
@@ -1370,13 +1376,13 @@
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="B50" s="1">
-        <v>42873</v>
+        <v>37463</v>
       </c>
       <c r="C50" s="1">
-        <v>42951</v>
+        <v>38286</v>
       </c>
       <c r="D50" t="s">
         <v>8</v>
@@ -1387,30 +1393,30 @@
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="B51" s="1">
-        <v>38413</v>
+        <v>39896</v>
       </c>
       <c r="C51" s="1">
-        <v>39146</v>
+        <v>41157</v>
       </c>
       <c r="D51" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="E51" s="2">
-        <v>11000000</v>
+        <v>0</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="B52" s="1">
-        <v>41032</v>
+        <v>40483</v>
       </c>
       <c r="C52" s="1">
-        <v>41255</v>
+        <v>40892</v>
       </c>
       <c r="D52" t="s">
         <v>8</v>
@@ -1421,30 +1427,30 @@
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>47</v>
+        <v>12</v>
       </c>
       <c r="B53" s="1">
-        <v>40214</v>
+        <v>39462</v>
       </c>
       <c r="C53" s="1">
-        <v>40890</v>
+        <v>40469</v>
       </c>
       <c r="D53" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="E53" s="2">
-        <v>0</v>
+        <v>3000000</v>
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
-        <v>47</v>
+        <v>12</v>
       </c>
       <c r="B54" s="1">
-        <v>38083</v>
+        <v>42968</v>
       </c>
       <c r="C54" s="1">
-        <v>38807</v>
+        <v>43004</v>
       </c>
       <c r="D54" t="s">
         <v>8</v>
@@ -1455,93 +1461,70 @@
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="B55" s="1">
-        <v>39896</v>
+        <v>40123</v>
       </c>
       <c r="C55" s="1">
-        <v>41157</v>
+        <v>41744</v>
       </c>
       <c r="D55" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="E55" s="2">
-        <v>0</v>
+        <v>35750000</v>
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="B56" s="1">
-        <v>37463</v>
+        <v>38497</v>
       </c>
       <c r="C56" s="1">
-        <v>38286</v>
+        <v>39325</v>
       </c>
       <c r="D56" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="E56" s="2">
-        <v>0</v>
+        <v>3500000</v>
       </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
-        <v>49</v>
+        <v>13</v>
       </c>
       <c r="B57" s="1">
-        <v>40483</v>
-      </c>
-      <c r="C57" s="1">
-        <v>40892</v>
+        <v>42999</v>
       </c>
       <c r="D57" t="s">
-        <v>8</v>
-      </c>
-      <c r="E57" s="2">
-        <v>0</v>
+        <v>11</v>
       </c>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
-        <v>50</v>
+        <v>14</v>
       </c>
       <c r="B58" s="1">
-        <v>40123</v>
+        <v>36826</v>
       </c>
       <c r="C58" s="1">
-        <v>41744</v>
+        <v>37797</v>
       </c>
       <c r="D58" t="s">
         <v>5</v>
       </c>
       <c r="E58" s="2">
-        <v>35750000</v>
-      </c>
-    </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A59" t="s">
-        <v>51</v>
-      </c>
-      <c r="B59" s="1">
-        <v>38497</v>
-      </c>
-      <c r="C59" s="1">
-        <v>39325</v>
-      </c>
-      <c r="D59" t="s">
-        <v>5</v>
-      </c>
-      <c r="E59" s="2">
-        <v>3500000</v>
+        <v>4000000</v>
       </c>
     </row>
   </sheetData>
   <autoFilter ref="A1:E1" xr:uid="{3C8B919C-4219-C142-BFB7-45AD54C78FA1}">
-    <sortState ref="A2:E32">
-      <sortCondition ref="A1:A32"/>
+    <sortState ref="A2:E58">
+      <sortCondition ref="A1:A58"/>
     </sortState>
   </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>